<commit_message>
set final training length, added final questions
</commit_message>
<xml_diff>
--- a/data/manipulation_tasks_easy.xlsx
+++ b/data/manipulation_tasks_easy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtcc\OneDrive\Desktop\rvl\llm_rl_for_manipulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B57057-AD8C-427F-B703-A2FD1B97AE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326D6F1F-68C3-44C3-97A3-9B6C61416E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="36">
   <si>
     <t>Text Question</t>
   </si>
@@ -57,16 +57,82 @@
     <t>(0.25,0.25,0.02)</t>
   </si>
   <si>
-    <t xml:space="preserve">Take the red block and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the blue block and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the green block and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the yellow block and move it to the position (0,0.375,0.02). </t>
+    <t>Take the blue block and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>(0,0.5,0.02)</t>
+  </si>
+  <si>
+    <t>Take the red block and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Take the green block and move it directly between the red and blue blocks</t>
+  </si>
+  <si>
+    <t>(0,0.25,0.02)</t>
+  </si>
+  <si>
+    <t>Take the yellow block and move it directly between the red and blue blocks</t>
+  </si>
+  <si>
+    <t>Pick up the blue block and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Pick up the red block and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Pick up the green block and move it directly between the red and blue blocks</t>
+  </si>
+  <si>
+    <t>Pick up the yellow block and move it directly between the red and blue blocks</t>
+  </si>
+  <si>
+    <t>Pick up the ocean-colored block and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of blood and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of celery and move it directly between the red and blue blocks</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of a lemon and move it directly between the red and blue blocks</t>
+  </si>
+  <si>
+    <t>Pick up the block that has the color of the sky and move it directly in between the forest colored block and the lemon colored block</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of a stop sign and move it directly in between the grass colored block and block with color closest to a banana</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of celery and move it directly between the heart colored block and the block with the same color as the Toronto Maple Leafs</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of a lemon and move it directly between the block with the color of a cardinal and the block with the color of the sky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the red block and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the blue block and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the green block and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the yellow block and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the block with a colour on the Canadian flag, and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the block that is the same colour as the ocean, and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the block that is the same colour as a traffic light that is telling cars to "go", and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the block that is the colour of the Saharah Desert, and move it to the position (0,0.375). </t>
   </si>
 </sst>
 </file>
@@ -384,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +465,7 @@
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,72 +482,484 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last training before project sub
</commit_message>
<xml_diff>
--- a/data/manipulation_tasks_easy.xlsx
+++ b/data/manipulation_tasks_easy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtcc\OneDrive\Desktop\rvl\llm_rl_for_manipulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B62A510-793B-494B-9E92-4622DD7FA133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3B9CCA-2BA9-4710-B48D-78FB0387AE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Text Question</t>
   </si>
@@ -57,67 +57,19 @@
     <t>(0.25,0.25,0.02)</t>
   </si>
   <si>
-    <t>(0,0.5,0.02)</t>
-  </si>
-  <si>
-    <t>Take the red block and move it directly in between the green and yellow blocks</t>
-  </si>
-  <si>
-    <t>Pick up the blue block and move it directly in between the green and yellow blocks</t>
-  </si>
-  <si>
-    <t>Pick up the red block and move it directly in between the green and yellow blocks</t>
-  </si>
-  <si>
-    <t>Pick up the ocean-colored block and move it directly in between the green and yellow blocks</t>
-  </si>
-  <si>
-    <t>Pick up the block that is the color of blood and move it directly in between the green and yellow blocks</t>
-  </si>
-  <si>
-    <t>Pick up the block that has the color of the sky and move it directly in between the forest colored block and the lemon colored block</t>
-  </si>
-  <si>
-    <t>Pick up the block that is the color of a stop sign and move it directly in between the grass colored block and block with color closest to a banana</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
-    <t xml:space="preserve">Take the red block and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the blue block and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the yellow block and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the block with a colour on the Canadian flag, and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the block that is the same colour as the ocean, and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the block that is the colour of the Saharah Desert, and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t>Take the blue block and move it directly in between the red and yellow blocks</t>
-  </si>
-  <si>
-    <t>Take the yellow block and move it directly between the green and blue blocks</t>
-  </si>
-  <si>
-    <t>(-0.25,0.375,0.02)</t>
-  </si>
-  <si>
-    <t>Pick up the yellow block and move it directly between the green and blue blocks</t>
-  </si>
-  <si>
-    <t>Pick up the block that is the color of a lemon and move it directly between the green and blue blocks</t>
-  </si>
-  <si>
-    <t>Pick up the block that is the color of a lemon and move it directly between the block with the color of grass and the block with the color of the sky</t>
+    <t xml:space="preserve">Take the red block and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the blue block and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the yellow block and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the green block and move it to the position (0,0.375). </t>
   </si>
 </sst>
 </file>
@@ -435,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,12 +419,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -492,7 +444,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -512,7 +464,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -532,10 +484,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -544,290 +496,10 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
setup for long training
</commit_message>
<xml_diff>
--- a/data/manipulation_tasks_easy.xlsx
+++ b/data/manipulation_tasks_easy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtcc\OneDrive\Desktop\rvl\llm_rl_for_manipulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3B9CCA-2BA9-4710-B48D-78FB0387AE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FCF91C-A196-49CC-89B5-5D6566AC0777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="31">
   <si>
     <t>Text Question</t>
   </si>
@@ -69,7 +69,55 @@
     <t xml:space="preserve">Take the yellow block and move it to the position (0,0.375). </t>
   </si>
   <si>
-    <t xml:space="preserve">Take the green block and move it to the position (0,0.375). </t>
+    <t xml:space="preserve">Take the block with a colour on the Canadian flag, and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the block that is the same colour as the ocean, and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the block that is the colour of the Saharah Desert, and move it to the position (0,0.375). </t>
+  </si>
+  <si>
+    <t>Take the blue block and move it directly in between the red and yellow blocks</t>
+  </si>
+  <si>
+    <t>(0,0.5,0.02)</t>
+  </si>
+  <si>
+    <t>Take the red block and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Take the yellow block and move it directly between the green and blue blocks</t>
+  </si>
+  <si>
+    <t>(-0.25,0.375,0.02)</t>
+  </si>
+  <si>
+    <t>Pick up the blue block and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Pick up the red block and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Pick up the yellow block and move it directly between the green and blue blocks</t>
+  </si>
+  <si>
+    <t>Pick up the ocean-colored block and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of blood and move it directly in between the green and yellow blocks</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of a lemon and move it directly between the green and blue blocks</t>
+  </si>
+  <si>
+    <t>Pick up the block that has the color of the sky and move it directly in between the forest colored block and the lemon colored block</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of a stop sign and move it directly in between the grass colored block and block with color closest to a banana</t>
+  </si>
+  <si>
+    <t>Pick up the block that is the color of a lemon and move it directly between the block with the color of grass and the block with the color of the sky</t>
   </si>
 </sst>
 </file>
@@ -387,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +535,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -496,10 +544,290 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="F5">
-        <v>1</v>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>